<commit_message>
Various changes to documentation and layout in application.
</commit_message>
<xml_diff>
--- a/Documentation/Group 2 - Burndown Chart.xlsx
+++ b/Documentation/Group 2 - Burndown Chart.xlsx
@@ -670,7 +670,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1950,7 +1950,7 @@
   <dimension ref="B1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2129,9 @@
       <c r="J5" s="12">
         <v>0</v>
       </c>
-      <c r="K5" s="13"/>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
       <c r="L5" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2199,10 +2201,12 @@
       <c r="J7" s="12">
         <v>1</v>
       </c>
-      <c r="K7" s="13"/>
+      <c r="K7" s="13">
+        <v>1</v>
+      </c>
       <c r="L7" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -2233,7 +2237,9 @@
       <c r="J8" s="12">
         <v>0</v>
       </c>
-      <c r="K8" s="13"/>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
       <c r="L8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2267,10 +2273,12 @@
       <c r="J9" s="12">
         <v>2</v>
       </c>
-      <c r="K9" s="13"/>
+      <c r="K9" s="13">
+        <v>2</v>
+      </c>
       <c r="L9" s="24">
         <f>SUM(D9:K9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2301,10 +2309,12 @@
       <c r="J10" s="9">
         <v>1</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="10">
+        <v>2</v>
+      </c>
       <c r="L10" s="19">
         <f>SUM(D10:K10)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2335,10 +2345,12 @@
       <c r="J11" s="9">
         <v>1</v>
       </c>
-      <c r="K11" s="10"/>
+      <c r="K11" s="10">
+        <v>1</v>
+      </c>
       <c r="L11" s="19">
         <f>SUM(D11:K11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -2379,7 +2391,7 @@
       </c>
       <c r="K12" s="15">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>